<commit_message>
updating documentation to reflect that OCA will be static for all FBI subscriptions
</commit_message>
<xml_diff>
--- a/adapters/fbi-electronic-biometric-transmission-specification-adapter/src/main/resources/documentation/Rap Back EBTS Mapping.xlsx
+++ b/adapters/fbi-electronic-biometric-transmission-specification-adapter/src/main/resources/documentation/Rap Back EBTS Mapping.xlsx
@@ -637,8 +637,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -687,7 +691,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -700,6 +704,8 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -712,6 +718,8 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1046,7 +1054,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1099,7 +1107,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" hidden="1">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1437,7 +1445,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" hidden="1">
+    <row r="25" spans="1:6" ht="30">
       <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45" hidden="1">
+    <row r="29" spans="1:6" ht="45">
       <c r="A29" s="2" t="s">
         <v>73</v>
       </c>
@@ -1677,7 +1685,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="45" hidden="1">
+    <row r="40" spans="1:6" ht="45">
       <c r="B40" s="2" t="s">
         <v>106</v>
       </c>
@@ -1687,8 +1695,8 @@
       <c r="D40" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>167</v>
+      <c r="E40" s="10" t="s">
+        <v>174</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>168</v>
@@ -1711,7 +1719,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>112</v>
       </c>
@@ -1747,7 +1755,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="45" hidden="1">
+    <row r="45" spans="1:6" ht="45">
       <c r="B45" s="2" t="s">
         <v>115</v>
       </c>
@@ -1798,10 +1806,11 @@
         <filter val="/submsg-doc:SubscriptionMessage/submsg-ext:Subject/nc20:PersonName/nc20:PersonGivenName"/>
         <filter val="/submsg-doc:SubscriptionMessage/submsg-ext:Subject/nc20:PersonName/nc20:PersonSurName"/>
         <filter val="/submsg-doc:SubscriptionMessage/submsg-ext:SubscriptionReasonCode"/>
-        <filter val="auto-generate"/>
+        <filter val="auto-generated"/>
+        <filter val="container node"/>
         <filter val="hardcoded in XSLT"/>
         <filter val="map to SID"/>
-        <filter val="probably can hardcode in XSLT"/>
+        <filter val="N/A"/>
         <filter val="set in XSLT, based on &quot;purpose&quot; of the subscription"/>
         <filter val="XSL param, make configurable and pass into XSLT"/>
       </filters>

</xml_diff>